<commit_message>
Add best practice and referenced projects
</commit_message>
<xml_diff>
--- a/codebase structure.xlsx
+++ b/codebase structure.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3A3067-899D-46E6-8791-ABA092BB29E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="1305" windowWidth="18225" windowHeight="12360"/>
+    <workbookView xWindow="-48" yWindow="0" windowWidth="18228" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,23 +15,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>This is a collaborative codebase for people to share their scripts and projects. The first part is stand-alone functions/notebooks that can be used for other projects (please include simple examples to demonstrate how to use it).  The second part is example projects that utilize one or more functions in the first part. The first part will reference the projects in the second part.</t>
   </si>
@@ -253,12 +243,15 @@
   </si>
   <si>
     <t>Meng Xia</t>
+  </si>
+  <si>
+    <t>0. Best practice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -431,6 +424,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,23 +705,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -743,7 +738,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -768,7 +763,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -777,30 +772,32 @@
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -809,422 +806,439 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>73</v>
       </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>61</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>10</v>
       </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>62</v>
-      </c>
-      <c r="B53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
       </c>
       <c r="D54" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>65</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>66</v>
       </c>
-      <c r="B56" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>67</v>
-      </c>
-      <c r="B57" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>68</v>
       </c>
       <c r="B58" t="s">
         <v>23</v>
       </c>
       <c r="D58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add notebook in 3, add link to projects
</commit_message>
<xml_diff>
--- a/codebase structure.xlsx
+++ b/codebase structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3A3067-899D-46E6-8791-ABA092BB29E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F93D05-C3C2-4FA5-8C41-90C49287A262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="0" windowWidth="18228" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18228" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
   <si>
     <t>This is a collaborative codebase for people to share their scripts and projects. The first part is stand-alone functions/notebooks that can be used for other projects (please include simple examples to demonstrate how to use it).  The second part is example projects that utilize one or more functions in the first part. The first part will reference the projects in the second part.</t>
   </si>
@@ -58,24 +58,12 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>1.3 Diagnosis and Procedure codes to embeddings</t>
-  </si>
-  <si>
-    <t>1.4 Vital signs</t>
-  </si>
-  <si>
     <t>Very basic, others can add</t>
   </si>
   <si>
-    <t>1.5 Lab results</t>
-  </si>
-  <si>
     <t>1.6 Medications</t>
   </si>
   <si>
-    <t>1.7 Doctor notes</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -115,48 +103,21 @@
     <t>P1</t>
   </si>
   <si>
-    <t>2.5 Observability estimation</t>
-  </si>
-  <si>
     <t>Mengying</t>
   </si>
   <si>
-    <t>2.6 Formatting sequence data in pytorch</t>
-  </si>
-  <si>
     <t>Elliot</t>
   </si>
   <si>
     <t>3. Modeling</t>
   </si>
   <si>
-    <t>3.1 Hyperparameter tuning (Optuna)</t>
-  </si>
-  <si>
-    <t>3.2 Multi-label Classification tutorial</t>
-  </si>
-  <si>
     <t>Yuqi</t>
   </si>
   <si>
-    <t>3.3 Multi-Label Classification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Qin) </t>
-  </si>
-  <si>
     <t>3.4 Conditional Multi-Label Classification</t>
   </si>
   <si>
-    <t>3.5 Pytorch Embedding models</t>
-  </si>
-  <si>
-    <t>3.6 Transfer Learning</t>
-  </si>
-  <si>
-    <t>3.7 Time-to-event (survival analysis) in pytorch</t>
-  </si>
-  <si>
     <t>4. NLP</t>
   </si>
   <si>
@@ -179,9 +140,6 @@
   </si>
   <si>
     <t>5.2 Bootstrapping</t>
-  </si>
-  <si>
-    <t>5.3 Stratifying metrics by subsets</t>
   </si>
   <si>
     <t>5.4 Forest plots</t>
@@ -230,22 +188,55 @@
     <t>P7 Longitudinal Missingness Embedding (TF/Keras)</t>
   </si>
   <si>
-    <t>3.8 Discrete Time Neural Survival Model</t>
-  </si>
-  <si>
     <t>Matt</t>
   </si>
   <si>
-    <t>4.4 LLM (GPT, BERT) finetuning and prediction</t>
-  </si>
-  <si>
-    <t>3.9 Contrastive Learning</t>
-  </si>
-  <si>
     <t>Meng Xia</t>
   </si>
   <si>
     <t>0. Best practice</t>
+  </si>
+  <si>
+    <t>3.3 Multi-Label Classification Tutorial</t>
+  </si>
+  <si>
+    <t>3.5 Discrete Time Neural Survival Model</t>
+  </si>
+  <si>
+    <t>2.5 Observability Estimation</t>
+  </si>
+  <si>
+    <t>2.6 Formatting Sequence Data in Pytorch</t>
+  </si>
+  <si>
+    <t>1.3 Diagnosis and Procedure codes to Embeddings</t>
+  </si>
+  <si>
+    <t>1.4 Vital Signs</t>
+  </si>
+  <si>
+    <t>1.5 Lab Results</t>
+  </si>
+  <si>
+    <t>1.7 Doctor Notes</t>
+  </si>
+  <si>
+    <t>3.2 Pytorch Embedding Models</t>
+  </si>
+  <si>
+    <t>3.1 Hyperparameter Tuning (Optuna)</t>
+  </si>
+  <si>
+    <t>4.4 LLM (GPT, BERT) Finetuning and Prediction</t>
+  </si>
+  <si>
+    <t>5.3 Stratifying Metrics by Subsets</t>
+  </si>
+  <si>
+    <t>3.6 Contrastive Learning</t>
+  </si>
+  <si>
+    <t>3.7 Transfer Learning</t>
   </si>
 </sst>
 </file>
@@ -385,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -424,8 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,17 +762,15 @@
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="18"/>
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -808,13 +795,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -822,34 +809,34 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -857,53 +844,53 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -911,18 +898,21 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -930,20 +920,23 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -951,29 +944,38 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -981,10 +983,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -992,253 +994,240 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
+      <c r="A32" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>45</v>
+      <c r="A34" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
+      <c r="A38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>18</v>
+      <c r="A39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>50</v>
+      <c r="A40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>54</v>
+      <c r="A44" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>56</v>
+      <c r="A46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
+      <c r="A50" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>61</v>
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>64</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D56" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>